<commit_message>
Adding final files prior to ISEF
</commit_message>
<xml_diff>
--- a/statistics/anova_tukey_summaries.xlsx
+++ b/statistics/anova_tukey_summaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronabraham/Documents/Science Fair /Grade 12/NMF_Biomarker_Identification_and_Diagnosis/statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F33402F8-136A-2B46-A318-26C2080F3F75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6CBA9E92-A39E-1B4F-BCE0-40D39FD214D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="960" windowWidth="26340" windowHeight="13920" xr2:uid="{34E42C34-2137-634A-B6DB-1D8B070EC2EC}"/>
   </bookViews>
@@ -570,7 +570,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -593,24 +593,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -619,9 +606,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -636,6 +620,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1399FFB-C3FC-F648-85E7-6B2F0040BE49}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -965,20 +965,20 @@
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="5"/>
+    <row r="1" spans="1:12">
+      <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -991,8 +991,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:12" ht="19">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1008,8 +1008,8 @@
         <v>0.86929999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="19">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:12" ht="19">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1025,8 +1025,8 @@
         <v>0.13980000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:12" ht="19">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1042,8 +1042,8 @@
         <v>0.84709999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:12" ht="19">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1059,8 +1059,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:12" ht="19">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1075,9 +1075,14 @@
       <c r="E7" s="3">
         <v>0.60709999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="7" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1092,9 +1097,14 @@
       <c r="E8" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="7" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1109,9 +1119,14 @@
       <c r="E9" s="3">
         <v>0.13320000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="19">
-      <c r="A10" s="6" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" ht="19">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1126,9 +1141,14 @@
       <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="19">
-      <c r="A11" s="6" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:12" ht="19">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1143,9 +1163,14 @@
       <c r="E11" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="19">
-      <c r="A12" s="6" t="s">
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" spans="1:12" ht="19">
+      <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1160,9 +1185,14 @@
       <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="6" t="s">
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1177,10 +1207,65 @@
       <c r="E13" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+    </row>
+    <row r="17" spans="8:12">
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+    </row>
+    <row r="18" spans="8:12">
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+    </row>
+    <row r="19" spans="8:12">
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="8:12">
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>